<commit_message>
create a pyqt app
</commit_message>
<xml_diff>
--- a/schedule/this_year/历史统计.xlsx
+++ b/schedule/this_year/历史统计.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="历史" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="历史" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -475,25 +475,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
@@ -506,28 +506,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -537,13 +537,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -552,10 +552,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -571,10 +571,10 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
         <v>100</v>
@@ -599,25 +599,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
         <v>100</v>
@@ -633,10 +633,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
         <v>100</v>
@@ -645,10 +645,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -673,16 +673,16 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9">
@@ -692,28 +692,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>2</v>
       </c>
       <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4</v>
+      </c>
+      <c r="I9" t="n">
         <v>50</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="n">
-        <v>100</v>
       </c>
     </row>
     <row r="10">
@@ -723,13 +723,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -738,10 +738,10 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -754,25 +754,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" t="n">
         <v>100</v>
@@ -785,28 +785,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -847,13 +847,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -878,13 +878,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -909,13 +909,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>

</xml_diff>